<commit_message>
Docs : supply.csv 오류 수정
</commit_message>
<xml_diff>
--- a/file/CSV/supply.xlsx
+++ b/file/CSV/supply.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="734">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="737">
   <si>
     <t>제품코드</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2288,6 +2288,18 @@
   </si>
   <si>
     <t>A101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D102</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D103</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2684,8 +2696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E657"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3672,7 +3684,7 @@
         <v>99</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>28</v>
+        <v>734</v>
       </c>
       <c r="C58" s="4">
         <v>43556.75</v>
@@ -3689,7 +3701,7 @@
         <v>100</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>29</v>
+        <v>735</v>
       </c>
       <c r="C59" s="4">
         <v>43556.75</v>
@@ -3706,7 +3718,7 @@
         <v>101</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>31</v>
+        <v>736</v>
       </c>
       <c r="C60" s="4">
         <v>43556.75</v>

</xml_diff>